<commit_message>
complete task 3 and 4
</commit_message>
<xml_diff>
--- a/Lab2.xlsx
+++ b/Lab2.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vyatsu-my.sharepoint.com/personal/stud115407_vyatsu_ru/Documents/Учеба/3 курс/6 семестр/Параллельное программирование/Lab2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="11_AD4DF75460589B3ACB7284402FDC6CAC5ADEDDA5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A33F899-4FD8-4E15-A58B-DFC72BA559E2}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="11_AD4DF75460589B3ACB7284402FDC6CAC5ADEDDA5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91C4C01F-A105-4718-ACAC-777AA53B765E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task1" sheetId="1" r:id="rId1"/>
     <sheet name="task2" sheetId="2" r:id="rId2"/>
     <sheet name="task3" sheetId="3" r:id="rId3"/>
+    <sheet name="task4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Размер вектора</t>
   </si>
@@ -212,10 +213,19 @@
     <t>2048</t>
   </si>
   <si>
-    <t>Двойные указатели</t>
-  </si>
-  <si>
-    <t>Одинарные указатели</t>
+    <t>Размер массива</t>
+  </si>
+  <si>
+    <t>10^6</t>
+  </si>
+  <si>
+    <t>10^8</t>
+  </si>
+  <si>
+    <t>10^9</t>
+  </si>
+  <si>
+    <t>2*10^9</t>
   </si>
 </sst>
 </file>
@@ -260,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -273,6 +283,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,17 +587,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -659,17 +679,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -739,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C54238-6649-4942-A9AB-54372F0795C6}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,125 +770,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="A2" s="5"/>
       <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A10" s="8"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A8:D8"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A11:A13 A4:A6" numberStoredAsText="1"/>
+    <ignoredError sqref="A3:A5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7339A022-0A64-48C4-BCB3-DEBBBA6F1416}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add cmake config and complete task 4
</commit_message>
<xml_diff>
--- a/Lab2.xlsx
+++ b/Lab2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vyatsu-my.sharepoint.com/personal/stud115407_vyatsu_ru/Documents/Учеба/3 курс/6 семестр/Параллельное программирование/Lab2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\term_6\parallel_programming\lab_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="11_AD4DF75460589B3ACB7284402FDC6CAC5ADEDDA5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91C4C01F-A105-4718-ACAC-777AA53B765E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2C1F0D-3B57-4406-9832-9E4F4316F672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14535" yWindow="7830" windowWidth="13215" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>Размер вектора</t>
   </si>
@@ -216,16 +216,100 @@
     <t>Размер массива</t>
   </si>
   <si>
-    <t>10^6</t>
-  </si>
-  <si>
-    <t>10^8</t>
-  </si>
-  <si>
-    <t>10^9</t>
-  </si>
-  <si>
-    <t>2*10^9</t>
+    <t>0.0141912</t>
+  </si>
+  <si>
+    <t>0.0141052</t>
+  </si>
+  <si>
+    <t>0.0699026</t>
+  </si>
+  <si>
+    <t>6.24055</t>
+  </si>
+  <si>
+    <t>1.39541</t>
+  </si>
+  <si>
+    <t>1.39876</t>
+  </si>
+  <si>
+    <t>14.4048</t>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+  </si>
+  <si>
+    <t>14.401</t>
+  </si>
+  <si>
+    <t>61.1282</t>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+  </si>
+  <si>
+    <t>0.127869</t>
+  </si>
+  <si>
+    <t>0.143609</t>
+  </si>
+  <si>
+    <t>0.655288</t>
+  </si>
+  <si>
+    <t>30.451</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6.73997</t>
+  </si>
+  <si>
+    <t>7.14446</t>
   </si>
 </sst>
 </file>
@@ -281,18 +365,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,7 +661,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,17 +671,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -667,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB9CF52-B81E-4723-B908-18E8FBFD4A26}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:D5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,17 +763,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -770,17 +854,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -816,19 +900,19 @@
       <c r="D5" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -865,71 +949,117 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7339A022-0A64-48C4-BCB3-DEBBBA6F1416}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -937,5 +1067,9 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A3 A4:A5 A7" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring and making report
</commit_message>
<xml_diff>
--- a/Lab2.xlsx
+++ b/Lab2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\term_6\parallel_programming\lab_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2C1F0D-3B57-4406-9832-9E4F4316F672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA03C533-0FC1-43CD-B7F7-46F173AEA45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14535" yWindow="7830" windowWidth="13215" windowHeight="12120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3780" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task1" sheetId="1" r:id="rId1"/>
@@ -372,10 +372,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -661,7 +661,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,17 +671,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB9CF52-B81E-4723-B908-18E8FBFD4A26}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,17 +763,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C54238-6649-4942-A9AB-54372F0795C6}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,17 +854,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
@@ -964,17 +964,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1031,13 +1031,13 @@
       <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactoring and completing task 3
</commit_message>
<xml_diff>
--- a/Lab2.xlsx
+++ b/Lab2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\term_6\parallel_programming\lab_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA03C533-0FC1-43CD-B7F7-46F173AEA45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDED92A-517A-4F6C-8841-FD85347C22F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3780" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>Размер вектора</t>
   </si>
@@ -310,6 +310,33 @@
   </si>
   <si>
     <t>7.14446</t>
+  </si>
+  <si>
+    <t>0.0176926</t>
+  </si>
+  <si>
+    <t>1.28419</t>
+  </si>
+  <si>
+    <t>1.37147</t>
+  </si>
+  <si>
+    <t>7.35719</t>
+  </si>
+  <si>
+    <t>7.73854</t>
+  </si>
+  <si>
+    <t>0.138595</t>
+  </si>
+  <si>
+    <t>2.02386</t>
+  </si>
+  <si>
+    <t>31.7538</t>
+  </si>
+  <si>
+    <t>31.4294</t>
   </si>
 </sst>
 </file>
@@ -661,7 +688,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,12 +871,14 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -879,25 +908,43 @@
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>

</xml_diff>